<commit_message>
calcolo collegi separato per ramo
</commit_message>
<xml_diff>
--- a/scenari/politiche_2027.xlsx
+++ b/scenari/politiche_2027.xlsx
@@ -8,21 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\forna\Repos\elezioni\scenari\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EF5D09B-ADCE-4BA3-B3DF-586889BE1E07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9776FF4E-3F6E-4A0F-92E7-F196F626E1D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="3855" windowWidth="19440" windowHeight="14880" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="liste_future" sheetId="1" r:id="rId1"/>
     <sheet name="coalizioni_future" sheetId="3" r:id="rId2"/>
     <sheet name="flussi_previsti" sheetId="2" r:id="rId3"/>
+    <sheet name="camera_candidati_uni" sheetId="4" r:id="rId4"/>
+    <sheet name="senato_candidati_uni" sheetId="6" r:id="rId5"/>
+    <sheet name="camera_candidati_pluri" sheetId="7" r:id="rId6"/>
+    <sheet name="senato_candidati_pluri" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="166">
   <si>
     <t>LISTA_FUTURA</t>
   </si>
@@ -387,9 +391,6 @@
     <t>AUTODETERMINATZIONE</t>
   </si>
   <si>
-    <t>DATA_DI_NASCITA</t>
-  </si>
-  <si>
     <t>Fratelli d'Italia</t>
   </si>
   <si>
@@ -478,6 +479,51 @@
   </si>
   <si>
     <t>#505050</t>
+  </si>
+  <si>
+    <t>MINORANZA</t>
+  </si>
+  <si>
+    <t>LISTA_MINORANZA</t>
+  </si>
+  <si>
+    <t>CIRCOSCRIZIONE</t>
+  </si>
+  <si>
+    <t>COLLEGIO_PLURINOMINALE</t>
+  </si>
+  <si>
+    <t>COLLEGIO_UNINOMINALE</t>
+  </si>
+  <si>
+    <t>COGNOME_CAND_UNI</t>
+  </si>
+  <si>
+    <t>NOME_CAND_UNI</t>
+  </si>
+  <si>
+    <t>DATA_NASCITA_CAND_UNI</t>
+  </si>
+  <si>
+    <t>Trentino-Alto Adige/Südtirol</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>COGNOME_CAND_PLURI</t>
+  </si>
+  <si>
+    <t>NOME_CAND_PLURI</t>
+  </si>
+  <si>
+    <t>DATA_NASCITA_CAND_PLURI</t>
+  </si>
+  <si>
+    <t>NUMERO_CANDIDATO</t>
+  </si>
+  <si>
+    <t>Trentino-Alto Adige</t>
   </si>
 </sst>
 </file>
@@ -524,13 +570,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -879,13 +926,13 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -901,101 +948,101 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B9" t="s">
         <v>131</v>
       </c>
-      <c r="B9" t="s">
-        <v>132</v>
-      </c>
       <c r="C9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>134</v>
+      </c>
+      <c r="B10" t="s">
         <v>135</v>
       </c>
-      <c r="B10" t="s">
-        <v>136</v>
-      </c>
       <c r="C10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1011,7 +1058,7 @@
         <v>59</v>
       </c>
       <c r="C12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -1021,68 +1068,64 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8AAC81F-9508-4537-B86C-3FF6E0644331}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>126</v>
       </c>
-      <c r="C2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>127</v>
-      </c>
-      <c r="C3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>132</v>
-      </c>
-      <c r="C4" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+      <c r="B4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>59</v>
       </c>
-      <c r="C5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>136</v>
-      </c>
-      <c r="C6" t="s">
-        <v>150</v>
+        <v>135</v>
+      </c>
+      <c r="B6" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -1094,8 +1137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="D126" sqref="D126"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C137" sqref="C137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1125,7 +1168,7 @@
         <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1156,7 +1199,7 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1173,7 +1216,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -1190,7 +1233,7 @@
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -1207,7 +1250,7 @@
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -1247,7 +1290,7 @@
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1261,7 +1304,7 @@
         <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -1278,13 +1321,13 @@
         <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E10">
         <v>0.5</v>
       </c>
       <c r="F10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1298,13 +1341,13 @@
         <v>16</v>
       </c>
       <c r="D11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E11">
         <v>0.5</v>
       </c>
       <c r="F11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1318,7 +1361,7 @@
         <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -1352,7 +1395,7 @@
         <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -1369,13 +1412,13 @@
         <v>20</v>
       </c>
       <c r="D15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E15">
         <v>0.5</v>
       </c>
       <c r="F15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1389,13 +1432,13 @@
         <v>20</v>
       </c>
       <c r="D16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E16">
         <v>0.5</v>
       </c>
       <c r="F16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1409,7 +1452,7 @@
         <v>21</v>
       </c>
       <c r="D17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -1477,7 +1520,7 @@
         <v>62</v>
       </c>
       <c r="D21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -1511,7 +1554,7 @@
         <v>64</v>
       </c>
       <c r="D23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -1545,7 +1588,7 @@
         <v>66</v>
       </c>
       <c r="D25" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -1749,7 +1792,7 @@
         <v>10</v>
       </c>
       <c r="D37" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E37">
         <v>1</v>
@@ -1766,7 +1809,7 @@
         <v>24</v>
       </c>
       <c r="D38" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E38">
         <v>1</v>
@@ -1783,7 +1826,7 @@
         <v>12</v>
       </c>
       <c r="D39" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E39">
         <v>1</v>
@@ -1800,7 +1843,7 @@
         <v>25</v>
       </c>
       <c r="D40" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E40">
         <v>1</v>
@@ -1817,7 +1860,7 @@
         <v>26</v>
       </c>
       <c r="D41" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E41">
         <v>1</v>
@@ -1834,7 +1877,7 @@
         <v>27</v>
       </c>
       <c r="D42" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E42">
         <v>1</v>
@@ -1851,7 +1894,7 @@
         <v>17</v>
       </c>
       <c r="D43" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E43">
         <v>1</v>
@@ -1868,7 +1911,7 @@
         <v>28</v>
       </c>
       <c r="D44" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E44">
         <v>1</v>
@@ -1885,7 +1928,7 @@
         <v>21</v>
       </c>
       <c r="D45" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E45">
         <v>1</v>
@@ -1902,7 +1945,7 @@
         <v>29</v>
       </c>
       <c r="D46" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E46">
         <v>1</v>
@@ -1936,7 +1979,7 @@
         <v>31</v>
       </c>
       <c r="D48" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E48">
         <v>1</v>
@@ -2021,7 +2064,7 @@
         <v>69</v>
       </c>
       <c r="D53" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E53">
         <v>1</v>
@@ -2208,7 +2251,7 @@
         <v>21</v>
       </c>
       <c r="D64" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E64">
         <v>1</v>
@@ -2225,7 +2268,7 @@
         <v>38</v>
       </c>
       <c r="D65" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E65">
         <v>1</v>
@@ -2259,7 +2302,7 @@
         <v>40</v>
       </c>
       <c r="D67" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E67">
         <v>1</v>
@@ -2276,7 +2319,7 @@
         <v>41</v>
       </c>
       <c r="D68" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E68">
         <v>1</v>
@@ -2293,7 +2336,7 @@
         <v>15</v>
       </c>
       <c r="D69" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E69">
         <v>1</v>
@@ -2327,7 +2370,7 @@
         <v>43</v>
       </c>
       <c r="D71" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E71">
         <v>1</v>
@@ -2361,7 +2404,7 @@
         <v>45</v>
       </c>
       <c r="D73" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E73">
         <v>1</v>
@@ -2378,7 +2421,7 @@
         <v>46</v>
       </c>
       <c r="D74" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E74">
         <v>1</v>
@@ -2395,7 +2438,7 @@
         <v>12</v>
       </c>
       <c r="D75" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E75">
         <v>1</v>
@@ -2480,7 +2523,7 @@
         <v>49</v>
       </c>
       <c r="D80" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E80">
         <v>1</v>
@@ -2497,7 +2540,7 @@
         <v>21</v>
       </c>
       <c r="D81" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E81">
         <v>1</v>
@@ -2514,7 +2557,7 @@
         <v>38</v>
       </c>
       <c r="D82" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E82">
         <v>1</v>
@@ -2531,13 +2574,13 @@
         <v>50</v>
       </c>
       <c r="D83" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E83">
         <v>0.5</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -2551,13 +2594,13 @@
         <v>50</v>
       </c>
       <c r="D84" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E84">
         <v>0.5</v>
       </c>
       <c r="F84" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2571,7 +2614,7 @@
         <v>41</v>
       </c>
       <c r="D85" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E85">
         <v>1</v>
@@ -2605,7 +2648,7 @@
         <v>52</v>
       </c>
       <c r="D87" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E87">
         <v>1</v>
@@ -2622,7 +2665,7 @@
         <v>15</v>
       </c>
       <c r="D88" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E88">
         <v>1</v>
@@ -2639,7 +2682,7 @@
         <v>27</v>
       </c>
       <c r="D89" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E89">
         <v>1</v>
@@ -2809,7 +2852,7 @@
         <v>21</v>
       </c>
       <c r="D99" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E99">
         <v>1</v>
@@ -2826,7 +2869,7 @@
         <v>15</v>
       </c>
       <c r="D100" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E100">
         <v>1</v>
@@ -2843,7 +2886,7 @@
         <v>87</v>
       </c>
       <c r="D101" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E101">
         <v>1</v>
@@ -2860,7 +2903,7 @@
         <v>40</v>
       </c>
       <c r="D102" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E102">
         <v>1</v>
@@ -2877,7 +2920,7 @@
         <v>88</v>
       </c>
       <c r="D103" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E103">
         <v>1</v>
@@ -2894,7 +2937,7 @@
         <v>89</v>
       </c>
       <c r="D104" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E104">
         <v>1</v>
@@ -2911,7 +2954,7 @@
         <v>90</v>
       </c>
       <c r="D105" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E105">
         <v>1</v>
@@ -2928,7 +2971,7 @@
         <v>91</v>
       </c>
       <c r="D106" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E106">
         <v>1</v>
@@ -2945,7 +2988,7 @@
         <v>92</v>
       </c>
       <c r="D107" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E107">
         <v>1</v>
@@ -2962,7 +3005,7 @@
         <v>12</v>
       </c>
       <c r="D108" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E108">
         <v>1</v>
@@ -2979,7 +3022,7 @@
         <v>41</v>
       </c>
       <c r="D109" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E109">
         <v>1</v>
@@ -2996,7 +3039,7 @@
         <v>11</v>
       </c>
       <c r="D110" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E110">
         <v>1</v>
@@ -3030,7 +3073,7 @@
         <v>19</v>
       </c>
       <c r="D112" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E112">
         <v>1</v>
@@ -3132,7 +3175,7 @@
         <v>110</v>
       </c>
       <c r="D118" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E118">
         <v>1</v>
@@ -3149,7 +3192,7 @@
         <v>111</v>
       </c>
       <c r="D119" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E119">
         <v>1</v>
@@ -3166,7 +3209,7 @@
         <v>112</v>
       </c>
       <c r="D120" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E120">
         <v>1</v>
@@ -3183,7 +3226,7 @@
         <v>113</v>
       </c>
       <c r="D121" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E121">
         <v>1</v>
@@ -3200,7 +3243,7 @@
         <v>114</v>
       </c>
       <c r="D122" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E122">
         <v>1</v>
@@ -3217,7 +3260,7 @@
         <v>115</v>
       </c>
       <c r="D123" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E123">
         <v>1</v>
@@ -3234,7 +3277,7 @@
         <v>116</v>
       </c>
       <c r="D124" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E124">
         <v>1</v>
@@ -3251,7 +3294,7 @@
         <v>117</v>
       </c>
       <c r="D125" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E125">
         <v>1</v>
@@ -3268,7 +3311,7 @@
         <v>118</v>
       </c>
       <c r="D126" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E126">
         <v>1</v>
@@ -3285,7 +3328,7 @@
         <v>119</v>
       </c>
       <c r="D127" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E127">
         <v>1</v>
@@ -3302,7 +3345,7 @@
         <v>94</v>
       </c>
       <c r="D128" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E128">
         <v>1</v>
@@ -3319,7 +3362,7 @@
         <v>95</v>
       </c>
       <c r="D129" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E129">
         <v>1</v>
@@ -3336,7 +3379,7 @@
         <v>96</v>
       </c>
       <c r="D130" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E130">
         <v>1</v>
@@ -3353,7 +3396,7 @@
         <v>97</v>
       </c>
       <c r="D131" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E131">
         <v>0.33</v>
@@ -3370,7 +3413,7 @@
         <v>97</v>
       </c>
       <c r="D132" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E132">
         <v>0.33</v>
@@ -3387,7 +3430,7 @@
         <v>97</v>
       </c>
       <c r="D133" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E133">
         <v>0.33</v>
@@ -3404,7 +3447,7 @@
         <v>98</v>
       </c>
       <c r="D134" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E134">
         <v>1</v>
@@ -3421,7 +3464,7 @@
         <v>99</v>
       </c>
       <c r="D135" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E135">
         <v>1</v>
@@ -3438,7 +3481,7 @@
         <v>21</v>
       </c>
       <c r="D136" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E136">
         <v>1</v>
@@ -3455,7 +3498,7 @@
         <v>100</v>
       </c>
       <c r="D137" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E137">
         <v>1</v>
@@ -3472,7 +3515,7 @@
         <v>101</v>
       </c>
       <c r="D138" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E138">
         <v>1</v>
@@ -3561,4 +3604,482 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B68449A-D3DF-4402-9A39-2D8FFCF92682}">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" t="s">
+        <v>159</v>
+      </c>
+      <c r="D5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBCD40B9-46AF-46B4-A447-A0B3FBBAFB86}">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21102282-00F0-46CE-98E1-245471DBADFA}">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C7" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>134</v>
+      </c>
+      <c r="C10" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" t="b">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>159</v>
+      </c>
+      <c r="D12" t="s">
+        <v>160</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69A3052C-A016-475B-9F75-C69E34BF0E99}">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C7" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>134</v>
+      </c>
+      <c r="C10" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" t="b">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>165</v>
+      </c>
+      <c r="D12" t="s">
+        <v>160</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>